<commit_message>
Added some calculations, added values to scheme and SWD interface
</commit_message>
<xml_diff>
--- a/calc.xlsx
+++ b/calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosa\Documents\PhotonGun\photongun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciek\Desktop\PhotonBlaster\photongun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A567BA9-466C-4208-BF69-5976CDED1EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580D3A8D-92EA-47BA-9BFF-086CEB6E0735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>R_SBOOSTB:</t>
   </si>
@@ -75,12 +75,72 @@
   </si>
   <si>
     <t>Delta_L:</t>
+  </si>
+  <si>
+    <t>L1 [H]</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>uH</t>
+  </si>
+  <si>
+    <t>mH</t>
+  </si>
+  <si>
+    <t>I_COILPEAK [A]:</t>
+  </si>
+  <si>
+    <t>I_MOSFET_MAX [A]:</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>I_MOSFET_RMS [A]:</t>
+  </si>
+  <si>
+    <t>P_RESISTIVE [W]:</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>DIODE</t>
+  </si>
+  <si>
+    <t>C_OUTPUT [F]:</t>
+  </si>
+  <si>
+    <t>mF</t>
+  </si>
+  <si>
+    <t>uF</t>
+  </si>
+  <si>
+    <t>Dynamic_LED_Res:</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>C_IN [F]:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,13 +185,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -668,6 +729,314 @@
         <a:xfrm>
           <a:off x="609600" y="9525000"/>
           <a:ext cx="2695951" cy="838317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>676723</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>85817</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obraz 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40C77B1F-1F74-BFEF-36AF-A76B3E50B7A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="10668000"/>
+          <a:ext cx="3210373" cy="657317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57512</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>66764</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Obraz 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{603652D5-D230-E7ED-E2A6-32A3AC974FE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="12192000"/>
+          <a:ext cx="2591162" cy="638264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66952</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>142945</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Obraz 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{478B862E-D534-2887-1ACF-ED1139E3C548}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="12973050"/>
+          <a:ext cx="1981477" cy="504895"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533828</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>95343</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Obraz 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56ACB06E-3357-1AFC-F8A4-C35C4C893DFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="13906500"/>
+          <a:ext cx="3067478" cy="666843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>391647</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>133</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Obraz 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53096F01-A2AE-684B-135F-B27F68631832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="15240000"/>
+          <a:ext cx="8040222" cy="952633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>877224</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>124078</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Obraz 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{040BD5D4-2125-1DA2-9229-E2DC7A34B578}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="17173575"/>
+          <a:ext cx="6620799" cy="1810003"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>305162</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>95350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Obraz 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E945CC7B-189E-EB7C-151D-82CDDDB870EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="20716875"/>
+          <a:ext cx="2591162" cy="714475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -942,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K53"/>
+  <dimension ref="B3:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +1361,7 @@
         <v>2.7272727272727271E-2</v>
       </c>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1000,8 +1369,11 @@
         <f>(J5-J4)/J5</f>
         <v>0.63636363636363635</v>
       </c>
-    </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1010,7 +1382,7 @@
         <v>9.1666666666666661</v>
       </c>
     </row>
-    <row r="32" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I32" s="1" t="s">
         <v>8</v>
       </c>
@@ -1066,18 +1438,179 @@
         <v>2.1212121212121211E-6</v>
       </c>
     </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J41" s="3">
+        <f>J40</f>
+        <v>2.1212121212121211E-6</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <f>J41*1000</f>
+        <v>2.121212121212121E-3</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <f>J42*1000</f>
+        <v>2.1212121212121211</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46">
+        <f>(K4-J24*(J16+0.1+0.1))*(J40/J53)</f>
+        <v>3.4121094667606288E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J47" s="3">
+        <f>J46</f>
+        <v>3.4121094667606288E-5</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <f>J47*1000</f>
+        <v>3.4121094667606287E-2</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <f>J48*1000</f>
+        <v>34.121094667606286</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J53">
         <f>0.1*((1-J20)/J37)*J24</f>
         <v>0.91489361702127669</v>
+      </c>
+    </row>
+    <row r="58" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J58">
+        <f>1.1*J24</f>
+        <v>10.083333333333334</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66">
+        <f>J20/(1-J20)*J3</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J69">
+        <f>SQRT(J20)/(1-J20)*J3</f>
+        <v>6.5812232905440906</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I74" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J74">
+        <f>J69*J69*0.1</f>
+        <v>4.3312499999999989</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I101" t="s">
+        <v>30</v>
+      </c>
+      <c r="J101">
+        <v>1</v>
+      </c>
+      <c r="K101" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J102">
+        <f>(J20*J3*0.1)/(300000*J3*0.1*J101)</f>
+        <v>2.1212121212121211E-6</v>
+      </c>
+    </row>
+    <row r="103" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="J103">
+        <f>J102*1000</f>
+        <v>2.121212121212121E-3</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="J104">
+        <f>J103*1000</f>
+        <v>2.1212121212121211</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I111" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J111">
+        <f>0.2*J24/(8*300000*0.1)</f>
+        <v>7.6388888888888884E-6</v>
+      </c>
+    </row>
+    <row r="112" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="J112">
+        <f>J111*1000</f>
+        <v>7.6388888888888886E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J113">
+        <f>J112*1000</f>
+        <v>7.6388888888888884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified calc and added TODO description to scheme
</commit_message>
<xml_diff>
--- a/calc.xlsx
+++ b/calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciek\Desktop\PhotonBlaster\photongun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosa\Documents\PhotonGun\photongun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580D3A8D-92EA-47BA-9BFF-086CEB6E0735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4265A6-9BE0-46A9-BA12-8141AC728432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>R_SBOOSTB:</t>
   </si>
@@ -132,6 +132,33 @@
   </si>
   <si>
     <t>C_IN [F]:</t>
+  </si>
+  <si>
+    <t>q = I * t</t>
+  </si>
+  <si>
+    <t>t=</t>
+  </si>
+  <si>
+    <t>I=</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>mC</t>
+  </si>
+  <si>
+    <t>uC</t>
+  </si>
+  <si>
+    <t>nC</t>
   </si>
 </sst>
 </file>
@@ -192,7 +219,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1311,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K113"/>
+  <dimension ref="B3:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J114" sqref="J114"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,10 +1634,92 @@
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:10" x14ac:dyDescent="0.25">
       <c r="J113">
         <f>J112*1000</f>
         <v>7.6388888888888884</v>
+      </c>
+    </row>
+    <row r="125" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <v>300000</v>
+      </c>
+      <c r="I125" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E126" t="s">
+        <v>34</v>
+      </c>
+      <c r="F126">
+        <f>1/F125</f>
+        <v>3.3333333333333333E-6</v>
+      </c>
+      <c r="G126" t="s">
+        <v>23</v>
+      </c>
+      <c r="H126" t="s">
+        <v>37</v>
+      </c>
+      <c r="I126">
+        <f>F126*F130</f>
+        <v>5.9999999999999995E-8</v>
+      </c>
+      <c r="J126" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <f>F126*1000</f>
+        <v>3.3333333333333331E-3</v>
+      </c>
+      <c r="G127" t="s">
+        <v>24</v>
+      </c>
+      <c r="I127">
+        <f>I126*1000</f>
+        <v>5.9999999999999995E-5</v>
+      </c>
+      <c r="J127" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <f>F127*1000</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="G128" t="s">
+        <v>25</v>
+      </c>
+      <c r="I128">
+        <f>I127*1000</f>
+        <v>0.06</v>
+      </c>
+      <c r="J128" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="129" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="I129">
+        <f>I128*1000</f>
+        <v>60</v>
+      </c>
+      <c r="J129" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="130" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>35</v>
+      </c>
+      <c r="F130">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G130" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>